<commit_message>
File Manager added and changed the Professions.xls and put it in a different folder Professions
</commit_message>
<xml_diff>
--- a/Output/output.xlsx
+++ b/Output/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,28 +479,23 @@
       <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Supervisor</t>
+          <t>supervisor</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>SGT University
-City:</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Rohtak</t>
-        </is>
-      </c>
+          <t>TRUONG LONG EXPORT -</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Current</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
@@ -508,25 +503,21 @@
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Health Care Executive</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>supervisor</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -534,25 +525,21 @@
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Nursing Home</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>supervisor</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>2014</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
@@ -561,105 +548,38 @@
     <row r="5">
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Health Care Executive</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>BP</t>
-        </is>
-      </c>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Pulse</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Heath Executive</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>DCM TEXTILE LTD</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Rohtak Institute of Engineering and Management
-City</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Institution</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>